<commit_message>
checked cuda, proposal update, added papers
</commit_message>
<xml_diff>
--- a/proposal/figures/Gantt_chart.xlsx
+++ b/proposal/figures/Gantt_chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\OneDrive - mail.uni-paderborn.de\Studium\Master\4. Semester\Master thesis\repository\proposal\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F372CE-7C54-45CF-B22A-6B6D8CD1FA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D11109-8BE9-4837-AB91-4F414896628D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{671A0ABF-FF7D-4556-B183-9345BF308A26}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{671A0ABF-FF7D-4556-B183-9345BF308A26}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -51,53 +51,59 @@
     <t>Further Research</t>
   </si>
   <si>
-    <t>Implementation</t>
-  </si>
-  <si>
     <t>Editing and re-writing master thesis</t>
-  </si>
-  <si>
-    <t>Milestone: Submission of final version of master thesis</t>
   </si>
   <si>
     <t>Corrections and rewriting</t>
   </si>
   <si>
-    <t>Writing chapters Evaluation + Summary + Discussion chapters</t>
-  </si>
-  <si>
     <t>Writing chapter Approach</t>
   </si>
   <si>
-    <t>Wiriting chapters Introduction + Related work + Bachground</t>
+    <t>Milestone: Submission Implementation</t>
   </si>
   <si>
-    <t>Prepare Presentation</t>
+    <t>Milestone: Finished quoting part</t>
   </si>
   <si>
-    <t>Milestone: presentation</t>
+    <t>Implementation of the score function</t>
   </si>
   <si>
-    <t>Milestone: Submission first version of master thesis</t>
+    <t>Implementation of Uncertainty Sampling</t>
   </si>
   <si>
-    <t>Writing the proposal</t>
+    <t>Implement Evaluation of the approach</t>
   </si>
   <si>
-    <t>Implement Prototype</t>
+    <t>Further Improvements and Refactoring</t>
   </si>
   <si>
-    <t>Milestone:Submission prototype</t>
+    <t>First adjustment to the original approach</t>
   </si>
   <si>
-    <t>Milestone: Submission Implementation</t>
+    <t>Milestone: First working version of UCGAN</t>
+  </si>
+  <si>
+    <t>Writing first three chapters</t>
+  </si>
+  <si>
+    <t>Writing last three chapters</t>
+  </si>
+  <si>
+    <t>Milestone: Submission final version</t>
+  </si>
+  <si>
+    <t>Milestone: Submission first version</t>
+  </si>
+  <si>
+    <t>Implementation of score fct components</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,14 +114,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -142,11 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -185,8 +182,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22240586966680137"/>
-          <c:y val="8.2449944930578119E-3"/>
+          <c:x val="0.22240583919949689"/>
+          <c:y val="9.3093360403091019E-2"/>
           <c:w val="0.73607853632230591"/>
           <c:h val="0.85901773550252425"/>
         </c:manualLayout>
@@ -219,107 +216,119 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$19</c:f>
+              <c:f>Tabelle1!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Milestone: Submission Implementation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Implementation</c:v>
+                  <c:v>Further Improvements and Refactoring</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Milestone:Submission prototype</c:v>
+                  <c:v>Implement Evaluation of the approach</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Implement Prototype</c:v>
+                  <c:v>Milestone: First working version of UCGAN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Implementation of Uncertainty Sampling</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Implementation of the score function</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Milestone: presentation</c:v>
+                  <c:v>Implementation of score fct components</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Prepare Presentation</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Milestone: Submission of final version of master thesis</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                  <c:v>First adjustment to the original approach</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Milestone: Submission final version</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Corrections and rewriting</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>Milestone: Submission first version of master thesis</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>Milestone: Submission first version</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Editing and re-writing master thesis</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>Writing chapters Evaluation + Summary + Discussion chapters</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>Writing last three chapters</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Writing chapter Approach</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>Wiriting chapters Introduction + Related work + Bachground</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
+                  <c:v>Milestone: Finished quoting part</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Writing first three chapters</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Further Research</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Writing the proposal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$B$2:$B$19</c:f>
+              <c:f>Tabelle1!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>44651</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>44635</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44607</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44607</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44562</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44545</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44515</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>44501</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>44500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>44486</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>44681</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>44652</c:v>
-                </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
                   <c:v>44651</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="11">
                   <c:v>44621</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="12">
                   <c:v>44620</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="13">
                   <c:v>44606</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>44562</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>44576</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>44531</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="16">
+                  <c:v>44530</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>44516</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="18">
                   <c:v>44501</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44470</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,7 +355,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:srgbClr val="002060"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -356,107 +365,119 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Tabelle1!$A$2:$A$19</c:f>
+              <c:f>Tabelle1!$A$2:$A$22</c:f>
               <c:strCache>
-                <c:ptCount val="17"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>Milestone: Submission Implementation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Implementation</c:v>
+                  <c:v>Further Improvements and Refactoring</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Milestone:Submission prototype</c:v>
+                  <c:v>Implement Evaluation of the approach</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Implement Prototype</c:v>
+                  <c:v>Milestone: First working version of UCGAN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Implementation of Uncertainty Sampling</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Implementation of the score function</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Milestone: presentation</c:v>
+                  <c:v>Implementation of score fct components</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Prepare Presentation</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Milestone: Submission of final version of master thesis</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                  <c:v>First adjustment to the original approach</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Milestone: Submission final version</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>Corrections and rewriting</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>Milestone: Submission first version of master thesis</c:v>
-                </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
+                  <c:v>Milestone: Submission first version</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>Editing and re-writing master thesis</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>Writing chapters Evaluation + Summary + Discussion chapters</c:v>
-                </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
+                  <c:v>Writing last three chapters</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>Writing chapter Approach</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>Wiriting chapters Introduction + Related work + Bachground</c:v>
-                </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="16">
+                  <c:v>Milestone: Finished quoting part</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Writing first three chapters</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>Further Research</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Writing the proposal</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Tabelle1!$D$2:$D$19</c:f>
+              <c:f>Tabelle1!$D$2:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>15</c:v>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>31</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="18">
                   <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -505,11 +526,14 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -535,8 +559,8 @@
         <c:axId val="331163344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="44685"/>
-          <c:min val="44470"/>
+          <c:max val="44655"/>
+          <c:min val="44501"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1193,15 +1217,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>54430</xdr:colOff>
+      <xdr:colOff>130630</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>174169</xdr:rowOff>
+      <xdr:rowOff>88443</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>576944</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>119743</xdr:rowOff>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1229,15 +1253,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1469573</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:colOff>1364798</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>96611</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>3091544</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>97972</xdr:rowOff>
+      <xdr:colOff>2986769</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>183697</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1252,8 +1276,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1469573" y="4027715"/>
-          <a:ext cx="1621971" cy="272143"/>
+          <a:off x="1364798" y="4716236"/>
+          <a:ext cx="1621971" cy="277586"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1282,7 +1306,7 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:rPr lang="de-DE" sz="1600" b="1"/>
             <a:t>Theoretical part</a:t>
           </a:r>
         </a:p>
@@ -1293,15 +1317,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>315686</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>43542</xdr:rowOff>
+      <xdr:colOff>106136</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2993571</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>163284</xdr:rowOff>
+      <xdr:colOff>2924175</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>10884</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1316,8 +1340,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="315686" y="7021285"/>
-          <a:ext cx="2677885" cy="304799"/>
+          <a:off x="106136" y="7558767"/>
+          <a:ext cx="2818039" cy="310242"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1346,9 +1370,349 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:rPr lang="de-DE" sz="1600" b="1"/>
             <a:t>Practical part/ Implementation</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Raute 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C96DAF43-E8DA-4C42-B399-0543BAF75B05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11953875" y="7134225"/>
+          <a:ext cx="171450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Raute 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A9FCE1A-5FF1-4D7A-8ED9-F40404B8D1BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10086975" y="6619875"/>
+          <a:ext cx="171450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Raute 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1972F864-6E9F-4ECD-8694-A25E26D43043}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11963400" y="9715500"/>
+          <a:ext cx="171450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Raute 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D955243-A51F-4C56-870B-1409957905AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648200" y="5581650"/>
+          <a:ext cx="171450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Raute 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35236969-0EE1-42CC-8F9A-BFA77A6B9945}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9296400" y="8905875"/>
+          <a:ext cx="171450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1654,18 +2018,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947CFA52-4BA1-4303-B450-ACF6C0DFA398}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1679,9 +2043,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>44651</v>
@@ -1694,220 +2058,257 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1">
-        <v>44501</v>
+        <v>44635</v>
       </c>
       <c r="C3" s="1">
         <v>44651</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D5" si="0">C3-B3+1</f>
-        <v>151</v>
+        <f t="shared" ref="D3:D7" si="0">C3-B3+1</f>
+        <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>44500</v>
+        <v>44607</v>
       </c>
       <c r="C4" s="1">
-        <v>44500</v>
+        <v>44634</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1">
-        <v>44486</v>
+        <v>44607</v>
       </c>
       <c r="C5" s="1">
-        <v>44500</v>
+        <v>44607</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="21" x14ac:dyDescent="0.4">
-      <c r="A6" s="3"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44562</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44606</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44545</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44561</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B8" s="1">
-        <v>44681</v>
+        <v>44515</v>
       </c>
       <c r="C8" s="1">
-        <v>44681</v>
+        <v>44545</v>
       </c>
       <c r="D8">
         <f>C8-B8+1</f>
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>44652</v>
+        <v>44501</v>
       </c>
       <c r="C9" s="1">
-        <v>44681</v>
+        <v>44514</v>
       </c>
       <c r="D9">
         <f>C9-B9+1</f>
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="1">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1">
         <v>44651</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="1">
         <v>44651</v>
-      </c>
-      <c r="D10">
-        <f>C10-B10+1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1">
-        <v>44621</v>
-      </c>
-      <c r="C11" s="1">
-        <v>44651</v>
-      </c>
-      <c r="D11">
-        <f>C11-B11+1</f>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1">
-        <v>44620</v>
-      </c>
-      <c r="C12" s="1">
-        <v>44620</v>
       </c>
       <c r="D12">
         <f>C12-B12+1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="1">
-        <v>44606</v>
+        <v>44621</v>
       </c>
       <c r="C13" s="1">
-        <v>44620</v>
+        <v>44651</v>
       </c>
       <c r="D13">
         <f>C13-B13+1</f>
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>44562</v>
+        <v>44620</v>
       </c>
       <c r="C14" s="1">
-        <v>44576</v>
+        <v>44620</v>
       </c>
       <c r="D14">
         <f>C14-B14+1</f>
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1">
-        <v>44531</v>
+        <v>44606</v>
       </c>
       <c r="C15" s="1">
-        <v>44561</v>
+        <v>44620</v>
       </c>
       <c r="D15">
         <f>C15-B15+1</f>
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>44516</v>
+        <v>44576</v>
       </c>
       <c r="C16" s="1">
-        <v>44530</v>
+        <v>44605</v>
       </c>
       <c r="D16">
         <f>C16-B16+1</f>
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1">
-        <v>44501</v>
+        <v>44531</v>
       </c>
       <c r="C17" s="1">
-        <v>44515</v>
+        <v>44576</v>
       </c>
       <c r="D17">
         <f>C17-B17+1</f>
-        <v>15</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1">
-        <v>44470</v>
+        <v>44530</v>
       </c>
       <c r="C18" s="1">
-        <v>44500</v>
+        <v>44530</v>
       </c>
       <c r="D18">
         <f>C18-B18+1</f>
-        <v>31</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44516</v>
+      </c>
+      <c r="C19" s="1">
+        <v>44530</v>
+      </c>
+      <c r="D19">
+        <f>C19-B19+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44501</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44515</v>
+      </c>
+      <c r="D20">
+        <f>C20-B20+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
proposal: Related work (uncertraintys sampling), Gantt-chart
</commit_message>
<xml_diff>
--- a/proposal/figures/Gantt_chart.xlsx
+++ b/proposal/figures/Gantt_chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\OneDrive\OneDrive - mail.uni-paderborn.de\Studium\Master\4. Semester\Master thesis\repository\proposal\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D11109-8BE9-4837-AB91-4F414896628D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE173D53-E1B7-4D2C-BBA0-2B44689E6EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{671A0ABF-FF7D-4556-B183-9345BF308A26}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{671A0ABF-FF7D-4556-B183-9345BF308A26}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -97,13 +97,58 @@
   </si>
   <si>
     <t>Implementation of score fct components</t>
+  </si>
+  <si>
+    <t>Milestone: Final structure of my approach is fixed</t>
+  </si>
+  <si>
+    <t>Writing chapter Implementation</t>
+  </si>
+  <si>
+    <t>Writing Evaluation, Summary and Discussion</t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Further research, writing first three chapters</t>
+  </si>
+  <si>
+    <t>Sprint 1</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
+  </si>
+  <si>
+    <t>Sprint 5</t>
+  </si>
+  <si>
+    <t>Implementation of simple first version</t>
+  </si>
+  <si>
+    <t>Development of further alternatives and improvements</t>
+  </si>
+  <si>
+    <t>Definition and implementation of the final approach</t>
+  </si>
+  <si>
+    <t>Further improvements and Refactoring</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,16 +164,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -136,20 +215,169 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -526,7 +754,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1217,15 +1445,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>130630</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>88443</xdr:rowOff>
+      <xdr:colOff>104126</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>114947</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>202096</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>93179</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1380,13 +1608,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>619125</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>28575</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
@@ -1448,13 +1676,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
@@ -1516,13 +1744,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -1585,15 +1813,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>164824</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>175177</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>336274</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>165653</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1608,7 +1836,75 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4648200" y="5581650"/>
+          <a:off x="4776581" y="5416412"/>
+          <a:ext cx="171450" cy="176006"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Raute 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35236969-0EE1-42CC-8F9A-BFA77A6B9945}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9296400" y="8905875"/>
           <a:ext cx="171450" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
@@ -1652,23 +1948,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>144946</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>29405</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>84483</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19881</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Raute 9">
+        <xdr:cNvPr id="13" name="Raute 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35236969-0EE1-42CC-8F9A-BFA77A6B9945}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CD8765F-8C32-4891-B90A-5BCF823C9ED5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1676,8 +1972,212 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9296400" y="8905875"/>
-          <a:ext cx="171450" cy="180975"/>
+          <a:off x="15139781" y="2129875"/>
+          <a:ext cx="171450" cy="176006"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>144946</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>16153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>84483</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>6628</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Raute 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6028C334-5921-4CAF-8025-107BFE8AD89F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15139781" y="3402083"/>
+          <a:ext cx="171450" cy="176006"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>151572</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>2900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>91109</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>178906</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Raute 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B212EE6E-CF05-46D9-A63B-E624E6901A26}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14218755" y="1732309"/>
+          <a:ext cx="171450" cy="176006"/>
+        </a:xfrm>
+        <a:prstGeom prst="diamond">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>158198</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9528</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>97735</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Raute 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D20F61B8-0FAB-43D9-BCA5-F5123F42467A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13297728" y="2838867"/>
+          <a:ext cx="171450" cy="176005"/>
         </a:xfrm>
         <a:prstGeom prst="diamond">
           <a:avLst/>
@@ -2018,18 +2518,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{947CFA52-4BA1-4303-B450-ACF6C0DFA398}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N39" sqref="N39"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2042,8 +2544,30 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
+      <c r="Y1" s="22"/>
+      <c r="Z1" s="22"/>
+      <c r="AA1" s="22"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2057,8 +2581,41 @@
         <f>C2-B2+1</f>
         <v>1</v>
       </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="21"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -2072,8 +2629,73 @@
         <f t="shared" ref="D3:D7" si="0">C3-B3+1</f>
         <v>17</v>
       </c>
+      <c r="E3" s="22"/>
+      <c r="F3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+      <c r="H3" s="6">
+        <v>2</v>
+      </c>
+      <c r="I3" s="6">
+        <v>3</v>
+      </c>
+      <c r="J3" s="7">
+        <v>4</v>
+      </c>
+      <c r="K3" s="6">
+        <v>5</v>
+      </c>
+      <c r="L3" s="6">
+        <v>6</v>
+      </c>
+      <c r="M3" s="6">
+        <v>7</v>
+      </c>
+      <c r="N3" s="7">
+        <v>8</v>
+      </c>
+      <c r="O3" s="6">
+        <v>9</v>
+      </c>
+      <c r="P3" s="6">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>11</v>
+      </c>
+      <c r="R3" s="7">
+        <v>12</v>
+      </c>
+      <c r="S3" s="6">
+        <v>13</v>
+      </c>
+      <c r="T3" s="6">
+        <v>14</v>
+      </c>
+      <c r="U3" s="6">
+        <v>15</v>
+      </c>
+      <c r="V3" s="7">
+        <v>16</v>
+      </c>
+      <c r="W3" s="6">
+        <v>17</v>
+      </c>
+      <c r="X3" s="6">
+        <v>18</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>19</v>
+      </c>
+      <c r="Z3" s="7">
+        <v>20</v>
+      </c>
+      <c r="AA3" s="21"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2087,8 +2709,33 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="21"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2102,8 +2749,33 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="E5" s="22"/>
+      <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="17"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="17"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="22"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2117,8 +2789,33 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="22"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2132,8 +2829,33 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="22"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -2147,8 +2869,33 @@
         <f>C8-B8+1</f>
         <v>31</v>
       </c>
+      <c r="E8" s="22"/>
+      <c r="F8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="16"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="16"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="22"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2159,19 +2906,91 @@
         <v>44514</v>
       </c>
       <c r="D9">
-        <f>C9-B9+1</f>
         <v>14</v>
       </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="16"/>
+      <c r="V9" s="17"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="4"/>
+      <c r="AA9" s="22"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="17"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
+      <c r="V10" s="17"/>
+      <c r="W10" s="16"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="16"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="22"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="18"/>
+      <c r="L11" s="18"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="18"/>
+      <c r="P11" s="18"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="20"/>
+      <c r="AA11" s="22"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2182,11 +3001,36 @@
         <v>44651</v>
       </c>
       <c r="D12">
-        <f>C12-B12+1</f>
+        <f t="shared" ref="D12:D20" si="1">C12-B12+1</f>
         <v>1</v>
       </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="16"/>
+      <c r="V12" s="17"/>
+      <c r="W12" s="16"/>
+      <c r="X12" s="16"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="22"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -2197,11 +3041,36 @@
         <v>44651</v>
       </c>
       <c r="D13">
-        <f>C13-B13+1</f>
+        <f t="shared" si="1"/>
         <v>31</v>
       </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="17"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="17"/>
+      <c r="S13" s="16"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="16"/>
+      <c r="V13" s="17"/>
+      <c r="W13" s="16"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="16"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="22"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -2212,11 +3081,36 @@
         <v>44620</v>
       </c>
       <c r="D14">
-        <f>C14-B14+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="E14" s="22"/>
+      <c r="F14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="16"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="16"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="16"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="16"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="22"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2227,11 +3121,36 @@
         <v>44620</v>
       </c>
       <c r="D15">
-        <f>C15-B15+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="17"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="16"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="16"/>
+      <c r="V15" s="17"/>
+      <c r="W15" s="16"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="16"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="22"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -2242,11 +3161,36 @@
         <v>44605</v>
       </c>
       <c r="D16">
-        <f>C16-B16+1</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
+      <c r="E16" s="22"/>
+      <c r="F16" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="16"/>
+      <c r="R16" s="17"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="16"/>
+      <c r="V16" s="17"/>
+      <c r="W16" s="16"/>
+      <c r="X16" s="16"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="22"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2257,11 +3201,36 @@
         <v>44576</v>
       </c>
       <c r="D17">
-        <f>C17-B17+1</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
+      <c r="E17" s="22"/>
+      <c r="F17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="16"/>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="16"/>
+      <c r="X17" s="16"/>
+      <c r="Y17" s="16"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="22"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -2272,11 +3241,36 @@
         <v>44530</v>
       </c>
       <c r="D18">
-        <f>C18-B18+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="E18" s="22"/>
+      <c r="F18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="16"/>
+      <c r="Q18" s="16"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="16"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="16"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="22"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2287,11 +3281,35 @@
         <v>44530</v>
       </c>
       <c r="D19">
-        <f>C19-B19+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="E19" s="22"/>
+      <c r="F19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="18"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="20"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -2302,11 +3320,34 @@
         <v>44515</v>
       </c>
       <c r="D20">
-        <f>C20-B20+1</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
+      <c r="E20" s="22"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="16"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="16"/>
+      <c r="Q20" s="16"/>
+      <c r="R20" s="16"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="16"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="22"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>

</xml_diff>